<commit_message>
add line connectNull flag to R
</commit_message>
<xml_diff>
--- a/updated_script/Graphtext_022820.xlsx
+++ b/updated_script/Graphtext_022820.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9906FAF-5F9B-0F4C-A969-DB4CAF2067D6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5960E4-05AE-034B-8201-F76D0F097C0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1600" yWindow="880" windowWidth="25600" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="641">
   <si>
     <t>section</t>
   </si>
@@ -1988,6 +1988,12 @@
   </si>
   <si>
     <t>Copyedit title/notes/source!!!</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>connectNull,wideSmallMultiple</t>
   </si>
 </sst>
 </file>
@@ -2505,9 +2511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE52" sqref="AE52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4961,7 +4967,7 @@
         <v>620</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>635</v>
+        <v>87</v>
       </c>
       <c r="I30" s="30" t="s">
         <v>44</v>
@@ -5049,7 +5055,7 @@
         <v>620</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>635</v>
+        <v>87</v>
       </c>
       <c r="I31" s="30" t="s">
         <v>44</v>
@@ -5140,7 +5146,7 @@
         <v>620</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>635</v>
+        <v>87</v>
       </c>
       <c r="I32" s="30" t="s">
         <v>44</v>
@@ -5231,7 +5237,7 @@
         <v>620</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>635</v>
+        <v>87</v>
       </c>
       <c r="I33" s="30" t="s">
         <v>44</v>
@@ -5319,7 +5325,7 @@
         <v>620</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>635</v>
+        <v>87</v>
       </c>
       <c r="I34" s="30" t="s">
         <v>44</v>
@@ -5410,7 +5416,7 @@
         <v>620</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="I35" s="30" t="s">
         <v>44</v>
@@ -5424,7 +5430,7 @@
       </c>
       <c r="M35" s="30"/>
       <c r="N35" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" s="30">
         <v>0</v>
@@ -5491,7 +5497,7 @@
         <v>620</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="I36" s="28" t="s">
         <v>44</v>
@@ -5505,7 +5511,7 @@
       </c>
       <c r="M36" s="28"/>
       <c r="N36" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="28">
         <v>0</v>
@@ -6869,7 +6875,9 @@
       <c r="AB52" s="28"/>
       <c r="AC52" s="28"/>
       <c r="AD52" s="28"/>
-      <c r="AE52" s="28"/>
+      <c r="AE52" s="38" t="s">
+        <v>640</v>
+      </c>
       <c r="AF52" s="28"/>
       <c r="AG52" s="28"/>
       <c r="AH52" s="28"/>

</xml_diff>